<commit_message>
Moved new classifier into java resources folder. Added per dataset training results.
</commit_message>
<xml_diff>
--- a/docs/datasets.xlsx
+++ b/docs/datasets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
   <si>
     <t>Dataset size</t>
   </si>
@@ -341,6 +341,75 @@
   </si>
   <si>
     <t>0:23</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Individual training performance (F1 at 20 epochs)</t>
+  </si>
+  <si>
+    <t>Individual training performance on orig DS (F1 at 20 epochs)</t>
+  </si>
+  <si>
+    <t>0.84 0.93 0.88
+0.76 0.55 0.64</t>
+  </si>
+  <si>
+    <t>0.84 0.92 0.88
+0.69 0.50 0.58</t>
+  </si>
+  <si>
+    <t>0.82 0.84 0.83
+0.64 0.60 0.62</t>
+  </si>
+  <si>
+    <t>0.80 0.94 0.86
+0.65 0.25 0.36</t>
+  </si>
+  <si>
+    <t>0.90 0.97 0.94
+0.80 0.55 0.65</t>
+  </si>
+  <si>
+    <t>0.84 0.94 0.89
+0.77 0.53 0.63</t>
+  </si>
+  <si>
+    <t>0.85 0.93 0.89
+0.76 0.56 0.65</t>
+  </si>
+  <si>
+    <t>0.83 0.90 0.86
+0.74 0.59 0.66</t>
+  </si>
+  <si>
+    <t>0.77 0.92 0.84
+0.76 0.47 0.58</t>
+  </si>
+  <si>
+    <t>0.89 0.89 0.89
+0.81 0.82 0.82</t>
+  </si>
+  <si>
+    <t>0.90 0.97 0.93
+0.70 0.40 0.51</t>
+  </si>
+  <si>
+    <t>0.86 0.97 0.91
+0.83 0.49 0.62</t>
+  </si>
+  <si>
+    <t>0.85 0.90 0.87
+0.76 0.67 0.71</t>
+  </si>
+  <si>
+    <t>0.82 0.90 0.86
+0.68 0.50 0.58</t>
+  </si>
+  <si>
+    <t>0.85 0.92 0.88
+0.62 0.43 0.50</t>
   </si>
 </sst>
 </file>
@@ -377,7 +446,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -827,11 +896,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -902,42 +1048,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -963,11 +1073,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1044,18 +1149,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1091,6 +1184,116 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1404,27 +1607,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="24" t="s">
+      <c r="D1" s="79"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="81" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1434,8 +1637,8 @@
       <c r="E2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="29"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="82"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="30">
       <c r="A3" s="5" t="s">
@@ -1610,469 +1813,552 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:F21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="48" customWidth="1"/>
-    <col min="4" max="4" width="16" style="49" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="50" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="16" style="34" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="35" customWidth="1"/>
+    <col min="8" max="9" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="24" t="s">
+      <c r="E1" s="103"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="105" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="59" t="s">
+      <c r="H1" s="83" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A2" s="99"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:7" ht="30">
-      <c r="A3" s="62" t="s">
+      <c r="G2" s="106"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85"/>
+    </row>
+    <row r="3" spans="1:9" ht="30">
+      <c r="A3" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="92" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30">
-      <c r="A4" s="63" t="s">
+      <c r="H3" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="73"/>
+    </row>
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="47"/>
-    </row>
-    <row r="5" spans="1:7" ht="30">
-      <c r="A5" s="63" t="s">
+      <c r="G4" s="93"/>
+      <c r="H4" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="107" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1">
+      <c r="A5" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="70" t="s">
+      <c r="E5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="47"/>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="63" t="s">
+      <c r="G5" s="93"/>
+      <c r="H5" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="107" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="F6" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="47"/>
-    </row>
-    <row r="7" spans="1:7" ht="30">
-      <c r="A7" s="63" t="s">
+      <c r="G6" s="93"/>
+      <c r="H6" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="74"/>
+    </row>
+    <row r="7" spans="1:9" ht="30">
+      <c r="A7" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="70" t="s">
+      <c r="F7" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="47"/>
-    </row>
-    <row r="8" spans="1:7" ht="45.75" thickBot="1">
-      <c r="A8" s="65" t="s">
+      <c r="G7" s="93"/>
+      <c r="H7" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="74"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" thickBot="1">
+      <c r="A8" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="69" t="s">
+      <c r="E8" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="47"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1">
-      <c r="A9" s="62" t="s">
+      <c r="G8" s="93"/>
+      <c r="H8" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="75"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1">
+      <c r="A9" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="72" t="s">
+      <c r="E9" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="74" t="s">
+      <c r="G9" s="94" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1">
-      <c r="A10" s="63" t="s">
+      <c r="H9" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="86" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1">
+      <c r="A10" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="70" t="s">
+      <c r="F10" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="75"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1">
-      <c r="A11" s="63" t="s">
+      <c r="G10" s="95"/>
+      <c r="H10" s="72" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" s="87"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1">
+      <c r="A11" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="F11" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="75"/>
-    </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1">
-      <c r="A12" s="63" t="s">
+      <c r="G11" s="95"/>
+      <c r="H11" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="87"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1">
+      <c r="A12" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="75"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1">
-      <c r="A13" s="63" t="s">
+      <c r="G12" s="95"/>
+      <c r="H12" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="87"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1">
+      <c r="A13" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="70" t="s">
+      <c r="F13" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="75"/>
-    </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1">
-      <c r="A14" s="63" t="s">
+      <c r="G13" s="95"/>
+      <c r="H13" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="87"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1">
+      <c r="A14" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="78" t="s">
+      <c r="D14" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="79" t="s">
+      <c r="F14" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="75"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1" thickBot="1">
-      <c r="A15" s="66" t="s">
+      <c r="G14" s="95"/>
+      <c r="H14" s="72" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="87"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1">
+      <c r="A15" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="80" t="s">
+      <c r="D15" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="76"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1">
-      <c r="A16" s="67" t="s">
+      <c r="G15" s="96"/>
+      <c r="H15" s="108" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="88"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1">
+      <c r="A16" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="85" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="77" t="s">
+      <c r="D16" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="97" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1">
-      <c r="A17" s="63" t="s">
+      <c r="H16" s="89" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="91" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" customHeight="1">
+      <c r="A17" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="75"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1">
-      <c r="A18" s="68" t="s">
+      <c r="D17" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="95"/>
+      <c r="H17" s="89"/>
+      <c r="I17" s="89"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" customHeight="1">
+      <c r="A18" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="75"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1">
-      <c r="A19" s="63" t="s">
+      <c r="D18" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="95"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" customHeight="1">
+      <c r="A19" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="75"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1">
-      <c r="A20" s="68" t="s">
+      <c r="D19" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="95"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="89"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1">
+      <c r="A20" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="87" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="88" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="75"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1" thickBot="1">
-      <c r="A21" s="66" t="s">
+      <c r="D20" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="95"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1" thickBot="1">
+      <c r="A21" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="76"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1"/>
-    <row r="23" spans="1:7" ht="30" customHeight="1"/>
-    <row r="24" spans="1:7" ht="30" customHeight="1"/>
-    <row r="25" spans="1:7" ht="30" customHeight="1"/>
-    <row r="26" spans="1:7" ht="30" customHeight="1"/>
+      <c r="D21" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="96"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" customHeight="1"/>
+    <row r="23" spans="1:9" ht="30" customHeight="1"/>
+    <row r="24" spans="1:9" ht="30" customHeight="1"/>
+    <row r="25" spans="1:9" ht="30" customHeight="1"/>
+    <row r="26" spans="1:9" ht="30" customHeight="1"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="13">
     <mergeCell ref="G3:G8"/>
     <mergeCell ref="G9:G15"/>
     <mergeCell ref="G16:G21"/>
@@ -2081,6 +2367,11 @@
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="I9:I15"/>
+    <mergeCell ref="H16:H21"/>
+    <mergeCell ref="I16:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added separation between damage amount and classification. Used regression model. UI changes.
</commit_message>
<xml_diff>
--- a/docs/datasets.xlsx
+++ b/docs/datasets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="120">
   <si>
     <t>Dataset size</t>
   </si>
@@ -410,6 +410,12 @@
   <si>
     <t>0.85 0.92 0.88
 0.62 0.43 0.50</t>
+  </si>
+  <si>
+    <t>Regression training (2 values) (MSE at 100 epochs)</t>
+  </si>
+  <si>
+    <t>Regression training (all values) (MSE at 100 epochs)</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -966,18 +972,49 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1191,18 +1228,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1219,33 +1250,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1289,11 +1293,68 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1607,27 +1668,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="77" t="s">
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="79" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1637,8 +1698,8 @@
       <c r="E2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="82"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="80"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="30">
       <c r="A3" s="5" t="s">
@@ -1813,53 +1874,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="33" customWidth="1"/>
-    <col min="4" max="4" width="16" style="34" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" style="34" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="33" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="34" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="34" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="34" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="35" hidden="1" customWidth="1"/>
     <col min="8" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="11" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="98" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="D1" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="103"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="105" t="s">
+      <c r="E1" s="92"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="83" t="s">
+      <c r="H1" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="I1" s="111" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A2" s="99"/>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
+      <c r="J1" s="96" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="96" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A2" s="88"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
       <c r="D2" s="44" t="s">
         <v>22</v>
       </c>
@@ -1869,11 +1937,13 @@
       <c r="F2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="106"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85"/>
-    </row>
-    <row r="3" spans="1:9" ht="30">
+      <c r="G2" s="95"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+    </row>
+    <row r="3" spans="1:11" ht="30">
       <c r="A3" s="47" t="s">
         <v>40</v>
       </c>
@@ -1892,15 +1962,17 @@
       <c r="F3" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="81" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="I3" s="73"/>
-    </row>
-    <row r="4" spans="1:9" ht="30">
+      <c r="I3" s="101"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+    </row>
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="48" t="s">
         <v>46</v>
       </c>
@@ -1919,15 +1991,17 @@
       <c r="F4" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="93"/>
+      <c r="G4" s="82"/>
       <c r="H4" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="107" t="s">
+      <c r="I4" s="102" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1">
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+    </row>
+    <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="A5" s="48" t="s">
         <v>43</v>
       </c>
@@ -1946,15 +2020,17 @@
       <c r="F5" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="93"/>
+      <c r="G5" s="82"/>
       <c r="H5" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="107" t="s">
+      <c r="I5" s="102" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="30">
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
+    </row>
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" s="48" t="s">
         <v>44</v>
       </c>
@@ -1973,13 +2049,15 @@
       <c r="F6" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="93"/>
+      <c r="G6" s="82"/>
       <c r="H6" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="I6" s="74"/>
-    </row>
-    <row r="7" spans="1:9" ht="30">
+      <c r="I6" s="103"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+    </row>
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="48" t="s">
         <v>45</v>
       </c>
@@ -1998,13 +2076,15 @@
       <c r="F7" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="93"/>
+      <c r="G7" s="82"/>
       <c r="H7" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="I7" s="74"/>
-    </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" thickBot="1">
+      <c r="I7" s="103"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="114"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A8" s="50" t="s">
         <v>47</v>
       </c>
@@ -2023,13 +2103,15 @@
       <c r="F8" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="93"/>
-      <c r="H8" s="76" t="s">
+      <c r="G8" s="82"/>
+      <c r="H8" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="I8" s="75"/>
-    </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1">
+      <c r="I8" s="104"/>
+      <c r="J8" s="115"/>
+      <c r="K8" s="115"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1">
       <c r="A9" s="47" t="s">
         <v>51</v>
       </c>
@@ -2048,17 +2130,19 @@
       <c r="F9" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="94" t="s">
+      <c r="G9" s="83" t="s">
         <v>67</v>
       </c>
       <c r="H9" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="86" t="s">
+      <c r="I9" s="105" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1">
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1">
       <c r="A10" s="48" t="s">
         <v>54</v>
       </c>
@@ -2077,13 +2161,15 @@
       <c r="F10" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="95"/>
+      <c r="G10" s="84"/>
       <c r="H10" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="I10" s="87"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1">
+      <c r="I10" s="106"/>
+      <c r="J10" s="114"/>
+      <c r="K10" s="114"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1">
       <c r="A11" s="48" t="s">
         <v>56</v>
       </c>
@@ -2102,13 +2188,15 @@
       <c r="F11" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="95"/>
+      <c r="G11" s="84"/>
       <c r="H11" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="87"/>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1">
+      <c r="I11" s="106"/>
+      <c r="J11" s="114"/>
+      <c r="K11" s="114"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="48" t="s">
         <v>59</v>
       </c>
@@ -2127,13 +2215,15 @@
       <c r="F12" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="95"/>
+      <c r="G12" s="84"/>
       <c r="H12" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="87"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1">
+      <c r="I12" s="106"/>
+      <c r="J12" s="114"/>
+      <c r="K12" s="114"/>
+    </row>
+    <row r="13" spans="1:11" ht="30" customHeight="1">
       <c r="A13" s="48" t="s">
         <v>61</v>
       </c>
@@ -2152,13 +2242,15 @@
       <c r="F13" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="95"/>
+      <c r="G13" s="84"/>
       <c r="H13" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="87"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1">
+      <c r="I13" s="106"/>
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" customHeight="1">
       <c r="A14" s="48" t="s">
         <v>63</v>
       </c>
@@ -2177,13 +2269,15 @@
       <c r="F14" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="95"/>
+      <c r="G14" s="84"/>
       <c r="H14" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="I14" s="87"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1">
+      <c r="I14" s="106"/>
+      <c r="J14" s="114"/>
+      <c r="K14" s="114"/>
+    </row>
+    <row r="15" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A15" s="51" t="s">
         <v>65</v>
       </c>
@@ -2202,13 +2296,17 @@
       <c r="F15" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="96"/>
-      <c r="H15" s="108" t="s">
+      <c r="G15" s="85"/>
+      <c r="H15" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="I15" s="88"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1">
+      <c r="I15" s="107"/>
+      <c r="J15" s="115">
+        <v>0.10413</v>
+      </c>
+      <c r="K15" s="115"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1">
       <c r="A16" s="52" t="s">
         <v>68</v>
       </c>
@@ -2227,17 +2325,19 @@
       <c r="F16" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="97" t="s">
+      <c r="G16" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="89" t="s">
+      <c r="H16" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="I16" s="91" t="s">
+      <c r="I16" s="108" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1">
+      <c r="J16" s="116"/>
+      <c r="K16" s="116"/>
+    </row>
+    <row r="17" spans="1:11" ht="30" customHeight="1">
       <c r="A17" s="48" t="s">
         <v>70</v>
       </c>
@@ -2256,11 +2356,13 @@
       <c r="F17" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="95"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="89"/>
-    </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1">
+      <c r="G17" s="84"/>
+      <c r="H17" s="99"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="114"/>
+      <c r="K17" s="114"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" customHeight="1">
       <c r="A18" s="53" t="s">
         <v>72</v>
       </c>
@@ -2279,11 +2381,13 @@
       <c r="F18" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="95"/>
-      <c r="H18" s="89"/>
-      <c r="I18" s="89"/>
-    </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1">
+      <c r="G18" s="84"/>
+      <c r="H18" s="99"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="114"/>
+      <c r="K18" s="114"/>
+    </row>
+    <row r="19" spans="1:11" ht="30" customHeight="1">
       <c r="A19" s="48" t="s">
         <v>74</v>
       </c>
@@ -2302,11 +2406,13 @@
       <c r="F19" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="95"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
-    </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1">
+      <c r="G19" s="84"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="114"/>
+      <c r="K19" s="114"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1">
       <c r="A20" s="53" t="s">
         <v>76</v>
       </c>
@@ -2325,11 +2431,13 @@
       <c r="F20" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="95"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-    </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" thickBot="1">
+      <c r="G20" s="84"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="114"/>
+      <c r="K20" s="114"/>
+    </row>
+    <row r="21" spans="1:11" ht="30" customHeight="1" thickBot="1">
       <c r="A21" s="51" t="s">
         <v>77</v>
       </c>
@@ -2348,17 +2456,26 @@
       <c r="F21" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="96"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="90"/>
-    </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1"/>
-    <row r="23" spans="1:9" ht="30" customHeight="1"/>
-    <row r="24" spans="1:9" ht="30" customHeight="1"/>
-    <row r="25" spans="1:9" ht="30" customHeight="1"/>
-    <row r="26" spans="1:9" ht="30" customHeight="1"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="115"/>
+      <c r="K21" s="115"/>
+    </row>
+    <row r="22" spans="1:11" ht="30" customHeight="1"/>
+    <row r="23" spans="1:11" ht="30" customHeight="1"/>
+    <row r="24" spans="1:11" ht="30" customHeight="1"/>
+    <row r="25" spans="1:11" ht="30" customHeight="1"/>
+    <row r="26" spans="1:11" ht="30" customHeight="1"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="I9:I15"/>
+    <mergeCell ref="H16:H21"/>
+    <mergeCell ref="I16:I21"/>
     <mergeCell ref="G3:G8"/>
     <mergeCell ref="G9:G15"/>
     <mergeCell ref="G16:G21"/>
@@ -2367,11 +2484,6 @@
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="I9:I15"/>
-    <mergeCell ref="H16:H21"/>
-    <mergeCell ref="I16:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>